<commit_message>
Thanh - Weekly task update
</commit_message>
<xml_diff>
--- a/Plan/PROJECTPLAN.xlsx
+++ b/Plan/PROJECTPLAN.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="110">
   <si>
     <t>No.</t>
   </si>
@@ -175,9 +175,6 @@
   </si>
   <si>
     <t>Draw flows for some processes</t>
-  </si>
-  <si>
-    <t>Waiting</t>
   </si>
   <si>
     <t>Read: how to make a project plan and making plan for 1st week</t>
@@ -348,30 +345,12 @@
     <t>Meeting client at personal lab in Thu Duc</t>
   </si>
   <si>
-    <t>Read prototype to classify users which is synchronize with source code</t>
-  </si>
-  <si>
     <t>Write document for presentation on Thursday</t>
   </si>
   <si>
     <t>CODE001</t>
   </si>
   <si>
-    <t>Coding task</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Code phân quyền nhân viên theo prototype </t>
-  </si>
-  <si>
-    <t>Tú</t>
-  </si>
-  <si>
-    <t>Duy, Tú</t>
-  </si>
-  <si>
-    <t>Review task 35</t>
-  </si>
-  <si>
     <t>1PM at Ho Con Rua</t>
   </si>
   <si>
@@ -394,6 +373,24 @@
   </si>
   <si>
     <t>Hoang, Tu, Phuong</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Form 14.01, add "Loai" column to the table</t>
+  </si>
+  <si>
+    <t>Form 14.03, add "Ky hieu mau" column to the table</t>
+  </si>
+  <si>
+    <t>Form 15.01, add "Nguoi giao", "Nguoi nhan", "Dien ten" columns to the table</t>
+  </si>
+  <si>
+    <t>Tinh tien, Bang bao gia</t>
+  </si>
+  <si>
+    <t>Form 19.01, 19.02</t>
   </si>
 </sst>
 </file>
@@ -653,39 +650,84 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -710,52 +752,7 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1064,8 +1061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66"/>
+    <sheetView tabSelected="1" topLeftCell="D35" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q44" sqref="Q44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1084,116 +1081,116 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="35" t="s">
+      <c r="B1" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="53" t="s">
+      <c r="E1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="52" t="s">
+      <c r="F1" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="47" t="s">
+      <c r="G1" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="49" t="s">
+      <c r="H1" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="I1" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="48" t="s">
+      <c r="J1" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="48"/>
-      <c r="L1" s="47" t="s">
+      <c r="K1" s="35"/>
+      <c r="L1" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
-      <c r="O1" s="35" t="s">
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="39" t="s">
+      <c r="P1" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="30"/>
+      <c r="Q1" s="46"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="46"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="42" t="s">
+      <c r="A2" s="33"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="36" t="s">
+      <c r="K2" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="34" t="s">
+      <c r="L2" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="38" t="s">
+      <c r="M2" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="41" t="s">
+      <c r="N2" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="36"/>
-      <c r="P2" s="40"/>
-      <c r="Q2" s="31"/>
+      <c r="O2" s="51"/>
+      <c r="P2" s="55"/>
+      <c r="Q2" s="47"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="34"/>
-      <c r="M3" s="38"/>
-      <c r="N3" s="41"/>
-      <c r="O3" s="36"/>
-      <c r="P3" s="40"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="53"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="51"/>
+      <c r="P3" s="55"/>
     </row>
     <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
-      <c r="O4" s="29"/>
-      <c r="P4" s="29"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="31"/>
+      <c r="P4" s="31"/>
     </row>
     <row r="5" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="21">
@@ -1206,7 +1203,7 @@
         <v>38</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E5" s="21" t="s">
         <v>23</v>
@@ -1217,32 +1214,32 @@
       <c r="G5" s="21">
         <v>6</v>
       </c>
-      <c r="H5" s="23">
+      <c r="H5" s="22">
         <v>1</v>
       </c>
       <c r="I5" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="24">
+      <c r="J5" s="23">
         <v>42686</v>
       </c>
-      <c r="K5" s="24">
+      <c r="K5" s="23">
         <v>42686</v>
       </c>
-      <c r="L5" s="24">
+      <c r="L5" s="23">
         <v>42686</v>
       </c>
-      <c r="M5" s="24">
+      <c r="M5" s="23">
         <v>42686</v>
       </c>
-      <c r="N5" s="24">
+      <c r="N5" s="23">
         <v>42686</v>
       </c>
       <c r="O5" s="21" t="s">
         <v>42</v>
       </c>
       <c r="P5" s="21" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -1250,13 +1247,13 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>15</v>
@@ -1298,16 +1295,16 @@
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="F7" s="1">
         <v>3</v>
@@ -1346,13 +1343,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>17</v>
@@ -1394,13 +1391,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="D9" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>19</v>
@@ -1436,68 +1433,68 @@
         <v>42</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="29"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="29"/>
-      <c r="M10" s="29"/>
-      <c r="N10" s="29"/>
-      <c r="O10" s="29"/>
-      <c r="P10" s="29"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="31"/>
+      <c r="O10" s="31"/>
+      <c r="P10" s="31"/>
     </row>
     <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="54" t="s">
-        <v>107</v>
-      </c>
-      <c r="B11" s="55"/>
-      <c r="C11" s="55"/>
-      <c r="D11" s="55"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="55"/>
-      <c r="G11" s="55"/>
-      <c r="H11" s="55"/>
-      <c r="I11" s="55"/>
-      <c r="J11" s="55"/>
-      <c r="K11" s="55"/>
-      <c r="L11" s="55"/>
-      <c r="M11" s="55"/>
-      <c r="N11" s="55"/>
-      <c r="O11" s="55"/>
-      <c r="P11" s="56"/>
+      <c r="A11" s="43" t="s">
+        <v>100</v>
+      </c>
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="44"/>
+      <c r="K11" s="44"/>
+      <c r="L11" s="44"/>
+      <c r="M11" s="44"/>
+      <c r="N11" s="44"/>
+      <c r="O11" s="44"/>
+      <c r="P11" s="45"/>
     </row>
     <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="43"/>
-      <c r="C12" s="43"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="43"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="43"/>
-      <c r="K12" s="43"/>
-      <c r="L12" s="43"/>
-      <c r="M12" s="43"/>
-      <c r="N12" s="43"/>
-      <c r="O12" s="43"/>
-      <c r="P12" s="32"/>
+      <c r="A12" s="56" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="56"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="56"/>
+      <c r="H12" s="56"/>
+      <c r="I12" s="56"/>
+      <c r="J12" s="56"/>
+      <c r="K12" s="56"/>
+      <c r="L12" s="56"/>
+      <c r="M12" s="56"/>
+      <c r="N12" s="56"/>
+      <c r="O12" s="56"/>
+      <c r="P12" s="30"/>
     </row>
     <row r="13" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -1510,7 +1507,7 @@
         <v>14</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>15</v>
@@ -1911,32 +1908,32 @@
       <c r="G21" s="21">
         <v>5</v>
       </c>
-      <c r="H21" s="23">
+      <c r="H21" s="22">
         <v>1</v>
       </c>
       <c r="I21" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="J21" s="24">
+      <c r="J21" s="23">
         <v>42699</v>
       </c>
-      <c r="K21" s="24">
-        <v>42704</v>
-      </c>
-      <c r="L21" s="24">
+      <c r="K21" s="23">
+        <v>42704</v>
+      </c>
+      <c r="L21" s="23">
         <v>42699</v>
       </c>
-      <c r="M21" s="24">
-        <v>42704</v>
-      </c>
-      <c r="N21" s="24">
+      <c r="M21" s="23">
+        <v>42704</v>
+      </c>
+      <c r="N21" s="23">
         <v>42704</v>
       </c>
       <c r="O21" s="21" t="s">
         <v>42</v>
       </c>
       <c r="P21" s="21" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1985,7 +1982,7 @@
       <c r="O22" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="P22" s="44" t="s">
+      <c r="P22" s="29" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2035,10 +2032,10 @@
       <c r="O23" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="P23" s="44"/>
+      <c r="P23" s="29"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="27">
+      <c r="A24" s="26">
         <v>17</v>
       </c>
       <c r="B24" s="20" t="s">
@@ -2059,58 +2056,58 @@
       <c r="G24" s="20"/>
       <c r="H24" s="20"/>
       <c r="I24" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="J24" s="28">
-        <v>42704</v>
-      </c>
-      <c r="K24" s="28">
-        <v>42704</v>
-      </c>
-      <c r="L24" s="28">
-        <v>42704</v>
-      </c>
-      <c r="M24" s="28">
+        <v>71</v>
+      </c>
+      <c r="J24" s="27">
+        <v>42704</v>
+      </c>
+      <c r="K24" s="27">
+        <v>42704</v>
+      </c>
+      <c r="L24" s="27">
+        <v>42704</v>
+      </c>
+      <c r="M24" s="27">
         <v>42704</v>
       </c>
       <c r="N24" s="20"/>
       <c r="O24" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="P24" s="44"/>
+        <v>70</v>
+      </c>
+      <c r="P24" s="29"/>
     </row>
     <row r="25" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="B25" s="29"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="29"/>
-      <c r="I25" s="29"/>
-      <c r="J25" s="29"/>
-      <c r="K25" s="29"/>
-      <c r="L25" s="29"/>
-      <c r="M25" s="29"/>
-      <c r="N25" s="29"/>
-      <c r="O25" s="29"/>
-      <c r="P25" s="29"/>
+      <c r="A25" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="31"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="31"/>
+      <c r="J25" s="31"/>
+      <c r="K25" s="31"/>
+      <c r="L25" s="31"/>
+      <c r="M25" s="31"/>
+      <c r="N25" s="31"/>
+      <c r="O25" s="31"/>
+      <c r="P25" s="31"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>18</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>17</v>
@@ -2158,7 +2155,7 @@
         <v>29</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>17</v>
@@ -2200,13 +2197,13 @@
         <v>20</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>29</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>17</v>
@@ -2248,13 +2245,13 @@
         <v>21</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>29</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>17</v>
@@ -2296,13 +2293,13 @@
         <v>22</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>29</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E30" s="8" t="s">
         <v>17</v>
@@ -2344,16 +2341,16 @@
         <v>23</v>
       </c>
       <c r="B31" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C31" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="C31" s="13" t="s">
-        <v>74</v>
-      </c>
       <c r="D31" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="E31" s="13" t="s">
         <v>80</v>
-      </c>
-      <c r="E31" s="13" t="s">
-        <v>81</v>
       </c>
       <c r="F31" s="13">
         <v>6</v>
@@ -2392,16 +2389,16 @@
         <v>24</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C32" s="10" t="s">
         <v>44</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F32" s="10">
         <v>8</v>
@@ -2440,13 +2437,13 @@
         <v>25</v>
       </c>
       <c r="B33" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="C33" s="16" t="s">
+      <c r="D33" s="16" t="s">
         <v>83</v>
-      </c>
-      <c r="D33" s="16" t="s">
-        <v>84</v>
       </c>
       <c r="E33" s="16" t="s">
         <v>18</v>
@@ -2461,7 +2458,7 @@
         <v>1</v>
       </c>
       <c r="I33" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J33" s="4">
         <v>42714</v>
@@ -2488,16 +2485,16 @@
         <v>26</v>
       </c>
       <c r="B34" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="D34" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="E34" s="13" t="s">
         <v>74</v>
-      </c>
-      <c r="D34" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="E34" s="13" t="s">
-        <v>75</v>
       </c>
       <c r="F34" s="13">
         <v>4</v>
@@ -2532,40 +2529,40 @@
       <c r="P34" s="13"/>
     </row>
     <row r="35" spans="1:16" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="B35" s="29"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="29"/>
-      <c r="H35" s="29"/>
-      <c r="I35" s="29"/>
-      <c r="J35" s="29"/>
-      <c r="K35" s="29"/>
-      <c r="L35" s="29"/>
-      <c r="M35" s="29"/>
-      <c r="N35" s="29"/>
-      <c r="O35" s="29"/>
-      <c r="P35" s="29"/>
+      <c r="A35" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="B35" s="31"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="31"/>
+      <c r="G35" s="31"/>
+      <c r="H35" s="31"/>
+      <c r="I35" s="31"/>
+      <c r="J35" s="31"/>
+      <c r="K35" s="31"/>
+      <c r="L35" s="31"/>
+      <c r="M35" s="31"/>
+      <c r="N35" s="31"/>
+      <c r="O35" s="31"/>
+      <c r="P35" s="31"/>
     </row>
     <row r="36" spans="1:16" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>27</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C36" s="13" t="s">
         <v>44</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E36" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F36" s="13">
         <v>2</v>
@@ -2598,7 +2595,7 @@
         <v>42</v>
       </c>
       <c r="P36" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -2606,13 +2603,13 @@
         <v>28</v>
       </c>
       <c r="B37" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="C37" s="13" t="s">
+      <c r="D37" s="13" t="s">
         <v>78</v>
-      </c>
-      <c r="D37" s="13" t="s">
-        <v>79</v>
       </c>
       <c r="E37" s="13" t="s">
         <v>16</v>
@@ -2654,13 +2651,13 @@
         <v>29</v>
       </c>
       <c r="B38" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C38" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="C38" s="13" t="s">
+      <c r="D38" s="13" t="s">
         <v>88</v>
-      </c>
-      <c r="D38" s="13" t="s">
-        <v>89</v>
       </c>
       <c r="E38" s="13" t="s">
         <v>19</v>
@@ -2689,8 +2686,12 @@
       <c r="M38" s="14">
         <v>42718</v>
       </c>
-      <c r="N38" s="14"/>
-      <c r="O38" s="13"/>
+      <c r="N38" s="14">
+        <v>42718</v>
+      </c>
+      <c r="O38" s="13" t="s">
+        <v>42</v>
+      </c>
       <c r="P38" s="13"/>
     </row>
     <row r="39" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -2698,13 +2699,13 @@
         <v>30</v>
       </c>
       <c r="B39" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C39" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="C39" s="13" t="s">
-        <v>74</v>
-      </c>
       <c r="D39" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E39" s="13" t="s">
         <v>16</v>
@@ -2749,10 +2750,10 @@
         <v>36</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D40" s="13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E40" s="13" t="s">
         <v>15</v>
@@ -2794,13 +2795,13 @@
         <v>32</v>
       </c>
       <c r="B41" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C41" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="C41" s="18" t="s">
-        <v>74</v>
-      </c>
       <c r="D41" s="18" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="E41" s="18" t="s">
         <v>16</v>
@@ -2808,10 +2809,14 @@
       <c r="F41" s="18">
         <v>3</v>
       </c>
-      <c r="G41" s="18"/>
-      <c r="H41" s="2"/>
+      <c r="G41" s="18">
+        <v>3</v>
+      </c>
+      <c r="H41" s="2">
+        <v>1</v>
+      </c>
       <c r="I41" s="18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="J41" s="14">
         <v>42718</v>
@@ -2825,12 +2830,16 @@
       <c r="M41" s="14">
         <v>42718</v>
       </c>
-      <c r="N41" s="14"/>
-      <c r="O41" s="18"/>
+      <c r="N41" s="14">
+        <v>42718</v>
+      </c>
+      <c r="O41" s="18" t="s">
+        <v>42</v>
+      </c>
       <c r="P41" s="18"/>
     </row>
     <row r="42" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="25">
+      <c r="A42" s="24">
         <v>33</v>
       </c>
       <c r="B42" s="21" t="s">
@@ -2840,7 +2849,7 @@
         <v>38</v>
       </c>
       <c r="D42" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E42" s="21" t="s">
         <v>23</v>
@@ -2851,52 +2860,52 @@
       <c r="G42" s="21">
         <v>5</v>
       </c>
-      <c r="H42" s="23">
+      <c r="H42" s="22">
         <v>1</v>
       </c>
       <c r="I42" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="J42" s="26">
+        <v>24</v>
+      </c>
+      <c r="J42" s="25">
         <v>42719</v>
       </c>
-      <c r="K42" s="26">
+      <c r="K42" s="25">
         <v>42719</v>
       </c>
-      <c r="L42" s="26">
+      <c r="L42" s="25">
         <v>42719</v>
       </c>
-      <c r="M42" s="26">
+      <c r="M42" s="25">
         <v>42719</v>
       </c>
-      <c r="N42" s="26">
+      <c r="N42" s="25">
         <v>42719</v>
       </c>
       <c r="O42" s="21" t="s">
         <v>42</v>
       </c>
       <c r="P42" s="21" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>34</v>
       </c>
-      <c r="B43" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C43" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D43" s="13" t="s">
+      <c r="B43" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="E43" s="13" t="s">
-        <v>101</v>
+      <c r="C43" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="D43" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="E43" s="28" t="s">
+        <v>19</v>
       </c>
       <c r="F43" s="13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G43" s="13"/>
       <c r="H43" s="2"/>
@@ -2904,16 +2913,16 @@
         <v>30</v>
       </c>
       <c r="J43" s="14">
-        <v>42718</v>
+        <v>42720</v>
       </c>
       <c r="K43" s="14">
-        <v>42718</v>
+        <v>42724</v>
       </c>
       <c r="L43" s="14">
-        <v>42718</v>
+        <v>42720</v>
       </c>
       <c r="M43" s="14">
-        <v>42718</v>
+        <v>42724</v>
       </c>
       <c r="N43" s="14"/>
       <c r="O43" s="13"/>
@@ -2923,114 +2932,158 @@
       <c r="A44" s="3">
         <v>35</v>
       </c>
-      <c r="B44" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="C44" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="D44" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="E44" s="18" t="s">
-        <v>17</v>
+      <c r="B44" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="C44" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="D44" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="E44" s="28" t="s">
+        <v>16</v>
       </c>
       <c r="F44" s="18">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G44" s="18"/>
       <c r="H44" s="2"/>
-      <c r="I44" s="22" t="s">
+      <c r="I44" s="28" t="s">
         <v>30</v>
       </c>
       <c r="J44" s="14">
-        <v>42718</v>
+        <v>42720</v>
       </c>
       <c r="K44" s="14">
-        <v>42719</v>
+        <v>42724</v>
       </c>
       <c r="L44" s="14">
-        <v>42718</v>
+        <v>42720</v>
       </c>
       <c r="M44" s="14">
-        <v>42719</v>
+        <v>42724</v>
       </c>
       <c r="N44" s="14"/>
       <c r="O44" s="18"/>
       <c r="P44" s="18"/>
     </row>
-    <row r="45" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>36</v>
       </c>
-      <c r="B45" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="C45" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="D45" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="E45" s="18" t="s">
-        <v>100</v>
+      <c r="B45" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="C45" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="D45" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="E45" s="28" t="s">
+        <v>15</v>
       </c>
       <c r="F45" s="18">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G45" s="18"/>
       <c r="H45" s="2"/>
-      <c r="I45" s="22" t="s">
+      <c r="I45" s="28" t="s">
         <v>30</v>
       </c>
       <c r="J45" s="14">
-        <v>42718</v>
+        <v>42720</v>
       </c>
       <c r="K45" s="14">
-        <v>42719</v>
+        <v>42724</v>
       </c>
       <c r="L45" s="14">
-        <v>42718</v>
+        <v>42720</v>
       </c>
       <c r="M45" s="14">
-        <v>42719</v>
+        <v>42724</v>
       </c>
       <c r="N45" s="14"/>
       <c r="O45" s="18"/>
       <c r="P45" s="18"/>
     </row>
     <row r="46" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="3"/>
-      <c r="B46" s="18"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="18"/>
+      <c r="A46" s="3">
+        <v>37</v>
+      </c>
+      <c r="B46" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="C46" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="D46" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="E46" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="F46" s="18">
+        <v>8</v>
+      </c>
       <c r="G46" s="18"/>
       <c r="H46" s="2"/>
-      <c r="I46" s="18"/>
-      <c r="J46" s="14"/>
-      <c r="K46" s="14"/>
-      <c r="L46" s="14"/>
-      <c r="M46" s="14"/>
+      <c r="I46" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="J46" s="14">
+        <v>42720</v>
+      </c>
+      <c r="K46" s="14">
+        <v>42724</v>
+      </c>
+      <c r="L46" s="14">
+        <v>42720</v>
+      </c>
+      <c r="M46" s="14">
+        <v>42724</v>
+      </c>
       <c r="N46" s="14"/>
       <c r="O46" s="18"/>
       <c r="P46" s="18"/>
     </row>
     <row r="47" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="3"/>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="18"/>
+      <c r="A47" s="3">
+        <v>38</v>
+      </c>
+      <c r="B47" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="C47" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="D47" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="E47" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="F47" s="18">
+        <v>8</v>
+      </c>
       <c r="G47" s="18"/>
       <c r="H47" s="2"/>
-      <c r="I47" s="18"/>
-      <c r="J47" s="14"/>
-      <c r="K47" s="14"/>
-      <c r="L47" s="14"/>
-      <c r="M47" s="14"/>
+      <c r="I47" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="J47" s="14">
+        <v>42720</v>
+      </c>
+      <c r="K47" s="14">
+        <v>42724</v>
+      </c>
+      <c r="L47" s="14">
+        <v>42720</v>
+      </c>
+      <c r="M47" s="14">
+        <v>42724</v>
+      </c>
       <c r="N47" s="14"/>
       <c r="O47" s="18"/>
       <c r="P47" s="18"/>
@@ -3109,16 +3162,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="P22:P24"/>
-    <mergeCell ref="A4:P4"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="H1:H3"/>
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="F1:F3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="A11:P11"/>
     <mergeCell ref="A35:P35"/>
     <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="A10:P10"/>
@@ -3135,6 +3178,16 @@
     <mergeCell ref="I1:I3"/>
     <mergeCell ref="A25:P25"/>
     <mergeCell ref="A12:P12"/>
+    <mergeCell ref="P22:P24"/>
+    <mergeCell ref="A4:P4"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="H1:H3"/>
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="A11:P11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Thanh - weekly update
</commit_message>
<xml_diff>
--- a/Plan/PROJECTPLAN.xlsx
+++ b/Plan/PROJECTPLAN.xlsx
@@ -677,15 +677,60 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -710,52 +755,7 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1064,8 +1064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M43" sqref="M43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1084,99 +1084,99 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="35" t="s">
+      <c r="B1" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="53" t="s">
+      <c r="E1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="52" t="s">
+      <c r="F1" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="47" t="s">
+      <c r="G1" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="49" t="s">
+      <c r="H1" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="I1" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="48" t="s">
+      <c r="J1" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="48"/>
-      <c r="L1" s="47" t="s">
+      <c r="K1" s="35"/>
+      <c r="L1" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
-      <c r="O1" s="35" t="s">
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="39" t="s">
+      <c r="P1" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="30"/>
+      <c r="Q1" s="46"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="46"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="42" t="s">
+      <c r="A2" s="33"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="36" t="s">
+      <c r="K2" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="34" t="s">
+      <c r="L2" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="38" t="s">
+      <c r="M2" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="41" t="s">
+      <c r="N2" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="36"/>
-      <c r="P2" s="40"/>
-      <c r="Q2" s="31"/>
+      <c r="O2" s="51"/>
+      <c r="P2" s="55"/>
+      <c r="Q2" s="47"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="34"/>
-      <c r="M3" s="38"/>
-      <c r="N3" s="41"/>
-      <c r="O3" s="36"/>
-      <c r="P3" s="40"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="53"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="51"/>
+      <c r="P3" s="55"/>
     </row>
     <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="31" t="s">
         <v>26</v>
       </c>
       <c r="B4" s="29"/>
@@ -1440,7 +1440,7 @@
       </c>
     </row>
     <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="31" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="29"/>
@@ -1460,44 +1460,44 @@
       <c r="P10" s="29"/>
     </row>
     <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="54" t="s">
+      <c r="A11" s="43" t="s">
         <v>100</v>
       </c>
-      <c r="B11" s="55"/>
-      <c r="C11" s="55"/>
-      <c r="D11" s="55"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="55"/>
-      <c r="G11" s="55"/>
-      <c r="H11" s="55"/>
-      <c r="I11" s="55"/>
-      <c r="J11" s="55"/>
-      <c r="K11" s="55"/>
-      <c r="L11" s="55"/>
-      <c r="M11" s="55"/>
-      <c r="N11" s="55"/>
-      <c r="O11" s="55"/>
-      <c r="P11" s="56"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="44"/>
+      <c r="K11" s="44"/>
+      <c r="L11" s="44"/>
+      <c r="M11" s="44"/>
+      <c r="N11" s="44"/>
+      <c r="O11" s="44"/>
+      <c r="P11" s="45"/>
     </row>
     <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="43"/>
-      <c r="C12" s="43"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="43"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="43"/>
-      <c r="K12" s="43"/>
-      <c r="L12" s="43"/>
-      <c r="M12" s="43"/>
-      <c r="N12" s="43"/>
-      <c r="O12" s="43"/>
-      <c r="P12" s="32"/>
+      <c r="B12" s="56"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="56"/>
+      <c r="H12" s="56"/>
+      <c r="I12" s="56"/>
+      <c r="J12" s="56"/>
+      <c r="K12" s="56"/>
+      <c r="L12" s="56"/>
+      <c r="M12" s="56"/>
+      <c r="N12" s="56"/>
+      <c r="O12" s="56"/>
+      <c r="P12" s="31"/>
     </row>
     <row r="13" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -1985,7 +1985,7 @@
       <c r="O22" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="P22" s="44" t="s">
+      <c r="P22" s="30" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2035,7 +2035,7 @@
       <c r="O23" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="P23" s="44"/>
+      <c r="P23" s="30"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="26">
@@ -2077,7 +2077,7 @@
       <c r="O24" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="P24" s="44"/>
+      <c r="P24" s="30"/>
     </row>
     <row r="25" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
@@ -2919,13 +2919,13 @@
         <v>42720</v>
       </c>
       <c r="K43" s="14">
-        <v>42724</v>
+        <v>42725</v>
       </c>
       <c r="L43" s="14">
         <v>42720</v>
       </c>
       <c r="M43" s="14">
-        <v>42724</v>
+        <v>42725</v>
       </c>
       <c r="N43" s="14"/>
       <c r="O43" s="13"/>
@@ -2959,13 +2959,13 @@
         <v>42720</v>
       </c>
       <c r="K44" s="14">
-        <v>42724</v>
+        <v>42725</v>
       </c>
       <c r="L44" s="14">
         <v>42720</v>
       </c>
       <c r="M44" s="14">
-        <v>42724</v>
+        <v>42725</v>
       </c>
       <c r="N44" s="14"/>
       <c r="O44" s="18"/>
@@ -2999,13 +2999,13 @@
         <v>42720</v>
       </c>
       <c r="K45" s="14">
-        <v>42724</v>
+        <v>42725</v>
       </c>
       <c r="L45" s="14">
         <v>42720</v>
       </c>
       <c r="M45" s="14">
-        <v>42724</v>
+        <v>42725</v>
       </c>
       <c r="N45" s="14"/>
       <c r="O45" s="18"/>
@@ -3039,13 +3039,13 @@
         <v>42720</v>
       </c>
       <c r="K46" s="14">
-        <v>42724</v>
+        <v>42725</v>
       </c>
       <c r="L46" s="14">
         <v>42720</v>
       </c>
       <c r="M46" s="14">
-        <v>42724</v>
+        <v>42725</v>
       </c>
       <c r="N46" s="14"/>
       <c r="O46" s="18"/>
@@ -3079,13 +3079,13 @@
         <v>42720</v>
       </c>
       <c r="K47" s="14">
-        <v>42724</v>
+        <v>42725</v>
       </c>
       <c r="L47" s="14">
         <v>42720</v>
       </c>
       <c r="M47" s="14">
-        <v>42724</v>
+        <v>42725</v>
       </c>
       <c r="N47" s="14"/>
       <c r="O47" s="18"/>
@@ -3167,18 +3167,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A48:P48"/>
-    <mergeCell ref="P22:P24"/>
-    <mergeCell ref="A4:P4"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="H1:H3"/>
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="F1:F3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="A11:P11"/>
-    <mergeCell ref="A35:P35"/>
     <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="A10:P10"/>
     <mergeCell ref="B1:B3"/>
@@ -3192,6 +3180,18 @@
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="J2:J3"/>
     <mergeCell ref="I1:I3"/>
+    <mergeCell ref="A48:P48"/>
+    <mergeCell ref="P22:P24"/>
+    <mergeCell ref="A4:P4"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="H1:H3"/>
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="A11:P11"/>
+    <mergeCell ref="A35:P35"/>
     <mergeCell ref="A25:P25"/>
     <mergeCell ref="A12:P12"/>
   </mergeCells>

</xml_diff>